<commit_message>
Added function to plot results
</commit_message>
<xml_diff>
--- a/Data/Elements.xlsx
+++ b/Data/Elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurivass/Desktop/OptimalTPI-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F582D9A6-9009-3649-A1F7-A0DE3A85F2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C9A9FB-9B19-2B40-8774-E0EC7F4B4546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16880" xr2:uid="{BD1B415B-D83E-2443-8E9A-9BE68552C4D1}"/>
   </bookViews>
@@ -128,15 +128,9 @@
     <t>Point(744 45)</t>
   </si>
   <si>
-    <t>LineString( 697 29, 721 29 )</t>
-  </si>
-  <si>
     <t>LineString( 788 36, 811 36 )</t>
   </si>
   <si>
-    <t>LineString( 695 36, 728 36 )</t>
-  </si>
-  <si>
     <t>LineString( 737 41, 771 41 )</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>Point(784 36)</t>
+  </si>
+  <si>
+    <t>LineString( 697 29, 722 29 )</t>
+  </si>
+  <si>
+    <t>LineString( 696 36, 720 36 )</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,7 +631,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -687,7 +687,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -699,7 +699,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -711,7 +711,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -723,7 +723,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -735,7 +735,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -747,7 +747,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -759,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -776,7 +776,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -793,7 +793,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>14</v>
@@ -810,7 +810,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>15</v>
@@ -827,7 +827,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -838,7 +838,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>